<commit_message>
prepare to merge into dev
</commit_message>
<xml_diff>
--- a/Silksong/Assets/Resources/AllDialogue.xlsx
+++ b/Silksong/Assets/Resources/AllDialogue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\魂灵之歌\Silksong\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FA03E4-657F-468E-B897-A27DD9E9EF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB5351-FA94-4A9B-A8E5-AA07C640B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="480" windowWidth="20790" windowHeight="14340" xr2:uid="{7A3AFAEE-5BB8-4897-9F8E-031E251E5F32}"/>
+    <workbookView xWindow="1680" yWindow="480" windowWidth="20790" windowHeight="14340" activeTab="1" xr2:uid="{7A3AFAEE-5BB8-4897-9F8E-031E251E5F32}"/>
   </bookViews>
   <sheets>
     <sheet name="plot" sheetId="1" r:id="rId1"/>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC2C54E-88A8-47F2-A3D5-D4908BD886CD}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -642,16 +642,16 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>6001</v>
+        <v>110001</v>
       </c>
       <c r="B2">
-        <v>6001</v>
+        <v>110001</v>
       </c>
       <c r="C2">
-        <v>6003</v>
+        <v>110003</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>1002</v>
@@ -662,13 +662,16 @@
       <c r="G2" t="s">
         <v>16</v>
       </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>6002</v>
+        <v>110002</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>1002</v>
@@ -676,10 +679,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>6003</v>
+        <v>110003</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1002</v>
@@ -687,16 +690,16 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>110001</v>
+        <v>105001</v>
       </c>
       <c r="B5">
-        <v>110001</v>
+        <v>105001</v>
       </c>
       <c r="C5">
-        <v>110003</v>
+        <v>105003</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1002</v>
@@ -707,16 +710,13 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>110002</v>
+        <v>105002</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>1002</v>
@@ -724,10 +724,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>110003</v>
+        <v>105003</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>1002</v>
@@ -735,16 +735,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>105001</v>
+        <v>6001</v>
       </c>
       <c r="B8">
-        <v>105001</v>
+        <v>6001</v>
       </c>
       <c r="C8">
-        <v>105003</v>
+        <v>6003</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>1002</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>105002</v>
+        <v>6002</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>1002</v>
@@ -769,10 +769,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>105003</v>
+        <v>6003</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>1002</v>
@@ -789,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A887DA09-5A7D-48CA-91F8-80BF08F72675}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>